<commit_message>
Rural areas and short names added (untested). Will test once all O3 data downloaded
</commit_message>
<xml_diff>
--- a/data/geo_data/trend_locations.xlsx
+++ b/data/geo_data/trend_locations.xlsx
@@ -22,11 +22,14 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="185" uniqueCount="162">
   <si>
     <t xml:space="preserve">Location</t>
   </si>
   <si>
+    <t xml:space="preserve">ShortName</t>
+  </si>
+  <si>
     <t xml:space="preserve">Latitude</t>
   </si>
   <si>
@@ -39,211 +42,472 @@
     <t xml:space="preserve">Albuquerque, NM</t>
   </si>
   <si>
+    <t xml:space="preserve">Albuquerque</t>
+  </si>
+  <si>
     <t xml:space="preserve">Atlanta, GA</t>
   </si>
   <si>
+    <t xml:space="preserve">Atlanta</t>
+  </si>
+  <si>
     <t xml:space="preserve">Bakersfield, CA</t>
   </si>
   <si>
+    <t xml:space="preserve">Bakersfield</t>
+  </si>
+  <si>
     <t xml:space="preserve">Boston, MA</t>
   </si>
   <si>
+    <t xml:space="preserve">Boston</t>
+  </si>
+  <si>
     <t xml:space="preserve">Charlotte, NC</t>
   </si>
   <si>
+    <t xml:space="preserve">Charlotte</t>
+  </si>
+  <si>
     <t xml:space="preserve">Chicago, IL</t>
   </si>
   <si>
+    <t xml:space="preserve">Chicago</t>
+  </si>
+  <si>
     <t xml:space="preserve">Cincinnati, OH</t>
   </si>
   <si>
+    <t xml:space="preserve">Cincinnati</t>
+  </si>
+  <si>
     <t xml:space="preserve">Cleveland, OH</t>
   </si>
   <si>
+    <t xml:space="preserve">Cleveland</t>
+  </si>
+  <si>
     <t xml:space="preserve">Columbus, OH</t>
   </si>
   <si>
+    <t xml:space="preserve">Columbus</t>
+  </si>
+  <si>
     <t xml:space="preserve">Dallas, TX</t>
   </si>
   <si>
+    <t xml:space="preserve">Dallas</t>
+  </si>
+  <si>
     <t xml:space="preserve">Denver, CO</t>
   </si>
   <si>
+    <t xml:space="preserve">Denver</t>
+  </si>
+  <si>
     <t xml:space="preserve">Detroit, MI</t>
   </si>
   <si>
+    <t xml:space="preserve">Detroit</t>
+  </si>
+  <si>
     <t xml:space="preserve">Fresno, CA</t>
   </si>
   <si>
+    <t xml:space="preserve">Fresno</t>
+  </si>
+  <si>
     <t xml:space="preserve">Houston, TX</t>
   </si>
   <si>
+    <t xml:space="preserve">Houston</t>
+  </si>
+  <si>
     <t xml:space="preserve">Indianapolis, IN</t>
   </si>
   <si>
+    <t xml:space="preserve">Indianapolis</t>
+  </si>
+  <si>
     <t xml:space="preserve">Jacksonville, FL</t>
   </si>
   <si>
+    <t xml:space="preserve">Jacksonville</t>
+  </si>
+  <si>
     <t xml:space="preserve">Kansas City, MO</t>
   </si>
   <si>
+    <t xml:space="preserve">Kansas City</t>
+  </si>
+  <si>
     <t xml:space="preserve">Knoxville, TN</t>
   </si>
   <si>
+    <t xml:space="preserve">Knoxville</t>
+  </si>
+  <si>
     <t xml:space="preserve">Las Vegas, NV</t>
   </si>
   <si>
+    <t xml:space="preserve">Las Vegas</t>
+  </si>
+  <si>
     <t xml:space="preserve">Los Angeles, CA</t>
   </si>
   <si>
+    <t xml:space="preserve">Los Angeles</t>
+  </si>
+  <si>
     <t xml:space="preserve">Memphis, TN</t>
   </si>
   <si>
+    <t xml:space="preserve">Memphis</t>
+  </si>
+  <si>
     <t xml:space="preserve">Miami, FL</t>
   </si>
   <si>
+    <t xml:space="preserve">Miami</t>
+  </si>
+  <si>
     <t xml:space="preserve">Minneapolis, MN</t>
   </si>
   <si>
+    <t xml:space="preserve">Minneapolis</t>
+  </si>
+  <si>
     <t xml:space="preserve">Montreal, QC</t>
   </si>
   <si>
+    <t xml:space="preserve">Montreal</t>
+  </si>
+  <si>
     <t xml:space="preserve">Nashville, TN</t>
   </si>
   <si>
+    <t xml:space="preserve">Nashville</t>
+  </si>
+  <si>
     <t xml:space="preserve">New Orleans, LA</t>
   </si>
   <si>
+    <t xml:space="preserve">New Orleans</t>
+  </si>
+  <si>
     <t xml:space="preserve">New York, NY</t>
   </si>
   <si>
+    <t xml:space="preserve">New York</t>
+  </si>
+  <si>
     <t xml:space="preserve">Omaha, NE</t>
   </si>
   <si>
+    <t xml:space="preserve">Omaha</t>
+  </si>
+  <si>
     <t xml:space="preserve">Orlando, FL</t>
   </si>
   <si>
+    <t xml:space="preserve">Orlando</t>
+  </si>
+  <si>
     <t xml:space="preserve">Philadelphia, PA</t>
   </si>
   <si>
+    <t xml:space="preserve">Philadelphia</t>
+  </si>
+  <si>
     <t xml:space="preserve">Phoenix, AZ</t>
   </si>
   <si>
+    <t xml:space="preserve">Phoenix</t>
+  </si>
+  <si>
     <t xml:space="preserve">Pittsburgh, PA</t>
   </si>
   <si>
+    <t xml:space="preserve">Pittsburgh</t>
+  </si>
+  <si>
     <t xml:space="preserve">Portland, OR</t>
   </si>
   <si>
+    <t xml:space="preserve">Portland</t>
+  </si>
+  <si>
     <t xml:space="preserve">Reno, NV</t>
   </si>
   <si>
+    <t xml:space="preserve">Reno</t>
+  </si>
+  <si>
     <t xml:space="preserve">Richmond, VA</t>
   </si>
   <si>
+    <t xml:space="preserve">Richmond</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sacramento, CA</t>
   </si>
   <si>
+    <t xml:space="preserve">Sacramento</t>
+  </si>
+  <si>
     <t xml:space="preserve">Salt Lake City, UT</t>
   </si>
   <si>
+    <t xml:space="preserve">Salt Lake City</t>
+  </si>
+  <si>
     <t xml:space="preserve">San Antonio, TX</t>
   </si>
   <si>
+    <t xml:space="preserve">San Antonio</t>
+  </si>
+  <si>
     <t xml:space="preserve">San Diego, CA</t>
   </si>
   <si>
+    <t xml:space="preserve">San Diego</t>
+  </si>
+  <si>
     <t xml:space="preserve">San Francisco, CA</t>
   </si>
   <si>
+    <t xml:space="preserve">San Francisco</t>
+  </si>
+  <si>
     <t xml:space="preserve">Seattle, WA</t>
   </si>
   <si>
+    <t xml:space="preserve">Seattle</t>
+  </si>
+  <si>
     <t xml:space="preserve">St Louis, MO</t>
   </si>
   <si>
+    <t xml:space="preserve">St Louis</t>
+  </si>
+  <si>
     <t xml:space="preserve">Tampa, FL</t>
   </si>
   <si>
+    <t xml:space="preserve">Tampa</t>
+  </si>
+  <si>
     <t xml:space="preserve">Toronto, ON</t>
   </si>
   <si>
+    <t xml:space="preserve">Toronto</t>
+  </si>
+  <si>
     <t xml:space="preserve">Tucson, AZ</t>
   </si>
   <si>
+    <t xml:space="preserve">Tucson</t>
+  </si>
+  <si>
     <t xml:space="preserve">Vancouver, BC</t>
   </si>
   <si>
+    <t xml:space="preserve">Vancouver</t>
+  </si>
+  <si>
     <t xml:space="preserve">Washington, DC</t>
   </si>
   <si>
+    <t xml:space="preserve">Washington DC</t>
+  </si>
+  <si>
     <t xml:space="preserve">Bruce Mansfield, PA</t>
   </si>
   <si>
+    <t xml:space="preserve">B Mansfield</t>
+  </si>
+  <si>
     <t xml:space="preserve">Cholla, AZ</t>
   </si>
   <si>
+    <t xml:space="preserve">Cholla</t>
+  </si>
+  <si>
     <t xml:space="preserve">Colstrip, MT</t>
   </si>
   <si>
+    <t xml:space="preserve">Colstrip</t>
+  </si>
+  <si>
     <t xml:space="preserve">Conemaugh, PA</t>
   </si>
   <si>
+    <t xml:space="preserve">Conemaugh</t>
+  </si>
+  <si>
     <t xml:space="preserve">Coronado Generating Station, AZ</t>
   </si>
   <si>
+    <t xml:space="preserve">Coronado</t>
+  </si>
+  <si>
     <t xml:space="preserve">Craig, CO</t>
   </si>
   <si>
+    <t xml:space="preserve">Craig</t>
+  </si>
+  <si>
     <t xml:space="preserve">Crystal River, FL</t>
   </si>
   <si>
+    <t xml:space="preserve">Crystal R</t>
+  </si>
+  <si>
     <t xml:space="preserve">Four Corners-San Juan, NM</t>
   </si>
   <si>
+    <t xml:space="preserve">Four Corners</t>
+  </si>
+  <si>
     <t xml:space="preserve">Gen J M Gavin, OH</t>
   </si>
   <si>
+    <t xml:space="preserve">JM Gavin</t>
+  </si>
+  <si>
     <t xml:space="preserve">Gibson, IN</t>
   </si>
   <si>
+    <t xml:space="preserve">Gibson</t>
+  </si>
+  <si>
     <t xml:space="preserve">Hatsfield Ferry Power Station, PA</t>
   </si>
   <si>
+    <t xml:space="preserve">Hatsfield</t>
+  </si>
+  <si>
     <t xml:space="preserve">Huntington, UT</t>
   </si>
   <si>
+    <t xml:space="preserve">Huntington</t>
+  </si>
+  <si>
     <t xml:space="preserve">Intermountain, UT</t>
   </si>
   <si>
+    <t xml:space="preserve">Intermountain</t>
+  </si>
+  <si>
     <t xml:space="preserve">Jim Bridger, WY</t>
   </si>
   <si>
+    <t xml:space="preserve">Jim Bridger</t>
+  </si>
+  <si>
     <t xml:space="preserve">JM Stuart, OH</t>
   </si>
   <si>
+    <t xml:space="preserve">JM Stuart</t>
+  </si>
+  <si>
     <t xml:space="preserve">Johnsonville, TN</t>
   </si>
   <si>
+    <t xml:space="preserve">Johnsonville</t>
+  </si>
+  <si>
     <t xml:space="preserve">Joppa Steam, IL</t>
   </si>
   <si>
+    <t xml:space="preserve">Joppa Steam</t>
+  </si>
+  <si>
     <t xml:space="preserve">Laramie River, WY</t>
   </si>
   <si>
+    <t xml:space="preserve">Laramie R</t>
+  </si>
+  <si>
     <t xml:space="preserve">Leland Olds, ND</t>
   </si>
   <si>
+    <t xml:space="preserve">Leland Olds</t>
+  </si>
+  <si>
     <t xml:space="preserve">Marshall, NC</t>
   </si>
   <si>
+    <t xml:space="preserve">Marshall</t>
+  </si>
+  <si>
     <t xml:space="preserve">Navajo Generating Station, AZ</t>
   </si>
   <si>
+    <t xml:space="preserve">Navajo</t>
+  </si>
+  <si>
     <t xml:space="preserve">Seminole, FL</t>
   </si>
   <si>
+    <t xml:space="preserve">Seminol</t>
+  </si>
+  <si>
     <t xml:space="preserve">Valmy, NV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Valmy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acacia</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Big Bend</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Crater Lake</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Death Valley</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grand Canyon</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Great Smokey Mountains</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Gt Smokey Mtn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hot Springs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Isle Royale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mt Rushmore</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Petrified Forest</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rural Alabama</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rural AL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shenandoah</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yellowstone</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Yosemite</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zion</t>
   </si>
 </sst>
 </file>
@@ -258,6 +522,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -339,16 +604,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D48"/>
+  <dimension ref="A1:E48"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C47" activeCellId="0" sqref="C47"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A15" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B49" activeCellId="0" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.8112244897959"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="16.6020408163265"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="13.9336734693878"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -364,662 +630,806 @@
       <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C2" s="0" t="n">
         <v>35.2</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="D2" s="0" t="n">
         <v>-106.55</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="E2" s="0" t="n">
         <v>30</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>5</v>
-      </c>
-      <c r="B3" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="0" t="n">
         <v>33.8</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="D3" s="0" t="n">
         <v>-84.35</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="E3" s="0" t="n">
         <v>35</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="0" t="n">
         <v>35.3</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="D4" s="0" t="n">
         <v>-119</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="E4" s="0" t="n">
         <v>25</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="0" t="n">
         <v>42.45</v>
       </c>
-      <c r="C5" s="0" t="n">
+      <c r="D5" s="0" t="n">
         <v>-71</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="E5" s="0" t="n">
         <v>30</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="C6" s="0" t="n">
         <v>35.25</v>
       </c>
-      <c r="C6" s="0" t="n">
+      <c r="D6" s="0" t="n">
         <v>-80.85</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="E6" s="0" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="0" t="n">
         <v>41.8</v>
       </c>
-      <c r="C7" s="0" t="n">
+      <c r="D7" s="0" t="n">
         <v>-87.7</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="E7" s="0" t="n">
         <v>60</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="B8" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="0" t="n">
         <v>39.1</v>
       </c>
-      <c r="C8" s="0" t="n">
+      <c r="D8" s="0" t="n">
         <v>-84.55</v>
       </c>
-      <c r="D8" s="0" t="n">
+      <c r="E8" s="0" t="n">
         <v>25</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="0" t="n">
         <v>41.45</v>
       </c>
-      <c r="C9" s="0" t="n">
+      <c r="D9" s="0" t="n">
         <v>-81.67</v>
       </c>
-      <c r="D9" s="0" t="n">
+      <c r="E9" s="0" t="n">
         <v>30</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>12</v>
-      </c>
-      <c r="B10" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="0" t="n">
         <v>40</v>
       </c>
-      <c r="C10" s="0" t="n">
+      <c r="D10" s="0" t="n">
         <v>-83.1</v>
       </c>
-      <c r="D10" s="0" t="n">
+      <c r="E10" s="0" t="n">
         <v>30</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>24</v>
+      </c>
+      <c r="C11" s="0" t="n">
         <v>32.85</v>
       </c>
-      <c r="C11" s="0" t="n">
+      <c r="D11" s="0" t="n">
         <v>-96.95</v>
       </c>
-      <c r="D11" s="0" t="n">
+      <c r="E11" s="0" t="n">
         <v>40</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>26</v>
+      </c>
+      <c r="C12" s="0" t="n">
         <v>39.75</v>
       </c>
-      <c r="C12" s="0" t="n">
+      <c r="D12" s="0" t="n">
         <v>-105</v>
       </c>
-      <c r="D12" s="0" t="n">
+      <c r="E12" s="0" t="n">
         <v>30</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="B13" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="0" t="n">
         <v>42.35</v>
       </c>
-      <c r="C13" s="0" t="n">
+      <c r="D13" s="0" t="n">
         <v>-83.1</v>
       </c>
-      <c r="D13" s="0" t="n">
+      <c r="E13" s="0" t="n">
         <v>45</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="B14" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="C14" s="0" t="n">
         <v>36.7</v>
       </c>
-      <c r="C14" s="0" t="n">
+      <c r="D14" s="0" t="n">
         <v>-119.75</v>
       </c>
-      <c r="D14" s="0" t="n">
+      <c r="E14" s="0" t="n">
         <v>25</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>17</v>
-      </c>
-      <c r="B15" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>32</v>
+      </c>
+      <c r="C15" s="0" t="n">
         <v>29.8</v>
       </c>
-      <c r="C15" s="0" t="n">
+      <c r="D15" s="0" t="n">
         <v>-95.25</v>
       </c>
-      <c r="D15" s="0" t="n">
+      <c r="E15" s="0" t="n">
         <v>30</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="C16" s="0" t="n">
         <v>39.8</v>
       </c>
-      <c r="C16" s="0" t="n">
+      <c r="D16" s="0" t="n">
         <v>-86.15</v>
       </c>
-      <c r="D16" s="0" t="n">
+      <c r="E16" s="0" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>19</v>
-      </c>
-      <c r="B17" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="C17" s="0" t="n">
         <v>30.45</v>
       </c>
-      <c r="C17" s="0" t="n">
+      <c r="D17" s="0" t="n">
         <v>-81.6</v>
       </c>
-      <c r="D17" s="0" t="n">
+      <c r="E17" s="0" t="n">
         <v>25</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="B18" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="C18" s="0" t="n">
         <v>39.15</v>
       </c>
-      <c r="C18" s="0" t="n">
+      <c r="D18" s="0" t="n">
         <v>-94.55</v>
       </c>
-      <c r="D18" s="0" t="n">
+      <c r="E18" s="0" t="n">
         <v>30</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="B19" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="C19" s="0" t="n">
         <v>35.95</v>
       </c>
-      <c r="C19" s="0" t="n">
+      <c r="D19" s="0" t="n">
         <v>-84</v>
       </c>
-      <c r="D19" s="0" t="n">
+      <c r="E19" s="0" t="n">
         <v>30</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="B20" s="0" t="n">
+        <v>41</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" s="0" t="n">
         <v>36.2</v>
       </c>
-      <c r="C20" s="0" t="n">
+      <c r="D20" s="0" t="n">
         <v>-115.2</v>
       </c>
-      <c r="D20" s="0" t="n">
+      <c r="E20" s="0" t="n">
         <v>25</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="B21" s="0" t="n">
+        <v>43</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" s="0" t="n">
         <v>34</v>
       </c>
-      <c r="C21" s="0" t="n">
+      <c r="D21" s="0" t="n">
         <v>-117.9</v>
       </c>
-      <c r="D21" s="0" t="n">
+      <c r="E21" s="0" t="n">
         <v>70</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="B22" s="0" t="n">
+        <v>45</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="C22" s="0" t="n">
         <v>35.1</v>
       </c>
-      <c r="C22" s="0" t="n">
+      <c r="D22" s="0" t="n">
         <v>-90.1</v>
       </c>
-      <c r="D22" s="0" t="n">
+      <c r="E22" s="0" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>25</v>
-      </c>
-      <c r="B23" s="0" t="n">
+        <v>47</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="C23" s="0" t="n">
         <v>26.05</v>
       </c>
-      <c r="C23" s="0" t="n">
+      <c r="D23" s="0" t="n">
         <v>-80.3</v>
       </c>
-      <c r="D23" s="0" t="n">
+      <c r="E23" s="0" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>26</v>
-      </c>
-      <c r="B24" s="0" t="n">
+        <v>49</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>50</v>
+      </c>
+      <c r="C24" s="0" t="n">
         <v>44.95</v>
       </c>
-      <c r="C24" s="0" t="n">
+      <c r="D24" s="0" t="n">
         <v>-93.25</v>
       </c>
-      <c r="D24" s="0" t="n">
+      <c r="E24" s="0" t="n">
         <v>30</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="B25" s="0" t="n">
+        <v>51</v>
+      </c>
+      <c r="B25" s="0" t="s">
+        <v>52</v>
+      </c>
+      <c r="C25" s="0" t="n">
         <v>45.6</v>
       </c>
-      <c r="C25" s="0" t="n">
+      <c r="D25" s="0" t="n">
         <v>-73.7</v>
       </c>
-      <c r="D25" s="0" t="n">
+      <c r="E25" s="0" t="n">
         <v>30</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="B26" s="0" t="n">
+        <v>53</v>
+      </c>
+      <c r="B26" s="0" t="s">
+        <v>54</v>
+      </c>
+      <c r="C26" s="0" t="n">
         <v>36.2</v>
       </c>
-      <c r="C26" s="0" t="n">
+      <c r="D26" s="0" t="n">
         <v>-86.6</v>
       </c>
-      <c r="D26" s="0" t="n">
+      <c r="E26" s="0" t="n">
         <v>30</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="B27" s="0" t="n">
+        <v>55</v>
+      </c>
+      <c r="B27" s="0" t="s">
+        <v>56</v>
+      </c>
+      <c r="C27" s="0" t="n">
         <v>30.05</v>
       </c>
-      <c r="C27" s="0" t="n">
+      <c r="D27" s="0" t="n">
         <v>-90.3</v>
       </c>
-      <c r="D27" s="0" t="n">
+      <c r="E27" s="0" t="n">
         <v>30</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="B28" s="0" t="n">
+        <v>57</v>
+      </c>
+      <c r="B28" s="0" t="s">
+        <v>58</v>
+      </c>
+      <c r="C28" s="0" t="n">
         <v>40.85</v>
       </c>
-      <c r="C28" s="0" t="n">
+      <c r="D28" s="0" t="n">
         <v>-73.7</v>
       </c>
-      <c r="D28" s="0" t="n">
+      <c r="E28" s="0" t="n">
         <v>70</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="B29" s="0" t="n">
+        <v>59</v>
+      </c>
+      <c r="B29" s="0" t="s">
+        <v>60</v>
+      </c>
+      <c r="C29" s="0" t="n">
         <v>41.3</v>
       </c>
-      <c r="C29" s="0" t="n">
+      <c r="D29" s="0" t="n">
         <v>-96.05</v>
       </c>
-      <c r="D29" s="0" t="n">
+      <c r="E29" s="0" t="n">
         <v>25</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="B30" s="0" t="n">
+        <v>61</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>62</v>
+      </c>
+      <c r="C30" s="0" t="n">
         <v>28.5</v>
       </c>
-      <c r="C30" s="0" t="n">
+      <c r="D30" s="0" t="n">
         <v>-81.3</v>
       </c>
-      <c r="D30" s="0" t="n">
+      <c r="E30" s="0" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
-        <v>33</v>
-      </c>
-      <c r="B31" s="0" t="n">
+        <v>63</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="C31" s="0" t="n">
         <v>40</v>
       </c>
-      <c r="C31" s="0" t="n">
+      <c r="D31" s="0" t="n">
         <v>-75.2</v>
       </c>
-      <c r="D31" s="0" t="n">
+      <c r="E31" s="0" t="n">
         <v>50</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="B32" s="0" t="n">
+        <v>65</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="C32" s="0" t="n">
         <v>33.6</v>
       </c>
-      <c r="C32" s="0" t="n">
+      <c r="D32" s="0" t="n">
         <v>-112</v>
       </c>
-      <c r="D32" s="0" t="n">
+      <c r="E32" s="0" t="n">
         <v>40</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="B33" s="0" t="n">
+        <v>67</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="C33" s="0" t="n">
         <v>40.4</v>
       </c>
-      <c r="C33" s="0" t="n">
+      <c r="D33" s="0" t="n">
         <v>-79.95</v>
       </c>
-      <c r="D33" s="0" t="n">
+      <c r="E33" s="0" t="n">
         <v>25</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="B34" s="0" t="n">
+        <v>69</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>70</v>
+      </c>
+      <c r="C34" s="0" t="n">
         <v>45.45</v>
       </c>
-      <c r="C34" s="0" t="n">
+      <c r="D34" s="0" t="n">
         <v>-122.55</v>
       </c>
-      <c r="D34" s="0" t="n">
+      <c r="E34" s="0" t="n">
         <v>30</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="B35" s="0" t="n">
+        <v>71</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>72</v>
+      </c>
+      <c r="C35" s="0" t="n">
         <v>39.55</v>
       </c>
-      <c r="C35" s="0" t="n">
+      <c r="D35" s="0" t="n">
         <v>-119.7</v>
       </c>
-      <c r="D35" s="0" t="n">
+      <c r="E35" s="0" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="B36" s="0" t="n">
+        <v>73</v>
+      </c>
+      <c r="B36" s="0" t="s">
+        <v>74</v>
+      </c>
+      <c r="C36" s="0" t="n">
         <v>37.4</v>
       </c>
-      <c r="C36" s="0" t="n">
+      <c r="D36" s="0" t="n">
         <v>-77.3</v>
       </c>
-      <c r="D36" s="0" t="n">
+      <c r="E36" s="0" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="B37" s="0" t="n">
+        <v>75</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>76</v>
+      </c>
+      <c r="C37" s="0" t="n">
         <v>38.65</v>
       </c>
-      <c r="C37" s="0" t="n">
+      <c r="D37" s="0" t="n">
         <v>-121.4</v>
       </c>
-      <c r="D37" s="0" t="n">
+      <c r="E37" s="0" t="n">
         <v>25</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>40</v>
-      </c>
-      <c r="B38" s="0" t="n">
+        <v>77</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>78</v>
+      </c>
+      <c r="C38" s="0" t="n">
         <v>40.7</v>
       </c>
-      <c r="C38" s="0" t="n">
+      <c r="D38" s="0" t="n">
         <v>-111.95</v>
       </c>
-      <c r="D38" s="0" t="n">
+      <c r="E38" s="0" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>41</v>
-      </c>
-      <c r="B39" s="0" t="n">
+        <v>79</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>80</v>
+      </c>
+      <c r="C39" s="0" t="n">
         <v>29.55</v>
       </c>
-      <c r="C39" s="0" t="n">
+      <c r="D39" s="0" t="n">
         <v>-98.45</v>
       </c>
-      <c r="D39" s="0" t="n">
+      <c r="E39" s="0" t="n">
         <v>30</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>42</v>
-      </c>
-      <c r="B40" s="0" t="n">
+        <v>81</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>82</v>
+      </c>
+      <c r="C40" s="0" t="n">
         <v>32.8</v>
       </c>
-      <c r="C40" s="0" t="n">
+      <c r="D40" s="0" t="n">
         <v>-117</v>
       </c>
-      <c r="D40" s="0" t="n">
+      <c r="E40" s="0" t="n">
         <v>25</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="B41" s="0" t="n">
+        <v>83</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="C41" s="0" t="n">
         <v>37.6</v>
       </c>
-      <c r="C41" s="0" t="n">
+      <c r="D41" s="0" t="n">
         <v>-122</v>
       </c>
-      <c r="D41" s="0" t="n">
+      <c r="E41" s="0" t="n">
         <v>40</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>44</v>
-      </c>
-      <c r="B42" s="0" t="n">
+        <v>85</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>86</v>
+      </c>
+      <c r="C42" s="0" t="n">
         <v>47.35</v>
       </c>
-      <c r="C42" s="0" t="n">
+      <c r="D42" s="0" t="n">
         <v>-122.25</v>
       </c>
-      <c r="D42" s="0" t="n">
+      <c r="E42" s="0" t="n">
         <v>50</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>45</v>
-      </c>
-      <c r="B43" s="0" t="n">
+        <v>87</v>
+      </c>
+      <c r="B43" s="0" t="s">
+        <v>88</v>
+      </c>
+      <c r="C43" s="0" t="n">
         <v>38.65</v>
       </c>
-      <c r="C43" s="0" t="n">
+      <c r="D43" s="0" t="n">
         <v>-90.35</v>
       </c>
-      <c r="D43" s="0" t="n">
+      <c r="E43" s="0" t="n">
         <v>30</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="B44" s="0" t="n">
+        <v>89</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="C44" s="0" t="n">
         <v>27.9</v>
       </c>
-      <c r="C44" s="0" t="n">
+      <c r="D44" s="0" t="n">
         <v>-82.4</v>
       </c>
-      <c r="D44" s="0" t="n">
+      <c r="E44" s="0" t="n">
         <v>30</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="B45" s="0" t="n">
+        <v>91</v>
+      </c>
+      <c r="B45" s="0" t="s">
+        <v>92</v>
+      </c>
+      <c r="C45" s="0" t="n">
         <v>43.7</v>
       </c>
-      <c r="C45" s="0" t="n">
+      <c r="D45" s="0" t="n">
         <v>-79.5</v>
       </c>
-      <c r="D45" s="0" t="n">
+      <c r="E45" s="0" t="n">
         <v>40</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>48</v>
-      </c>
-      <c r="B46" s="0" t="n">
+        <v>93</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>94</v>
+      </c>
+      <c r="C46" s="0" t="n">
         <v>32.25</v>
       </c>
-      <c r="C46" s="0" t="n">
+      <c r="D46" s="0" t="n">
         <v>-110.85</v>
       </c>
-      <c r="D46" s="0" t="n">
+      <c r="E46" s="0" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>49</v>
-      </c>
-      <c r="B47" s="0" t="n">
+        <v>95</v>
+      </c>
+      <c r="B47" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="C47" s="0" t="n">
         <v>49.25</v>
       </c>
-      <c r="C47" s="0" t="n">
+      <c r="D47" s="0" t="n">
         <v>-122.85</v>
       </c>
-      <c r="D47" s="0" t="n">
+      <c r="E47" s="0" t="n">
         <v>25</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>50</v>
-      </c>
-      <c r="B48" s="0" t="n">
+        <v>97</v>
+      </c>
+      <c r="B48" s="0" t="s">
+        <v>98</v>
+      </c>
+      <c r="C48" s="0" t="n">
         <v>39.15</v>
       </c>
-      <c r="C48" s="0" t="n">
+      <c r="D48" s="0" t="n">
         <v>-76.8</v>
       </c>
-      <c r="D48" s="0" t="n">
+      <c r="E48" s="0" t="n">
         <v>50</v>
       </c>
     </row>
@@ -1039,16 +1449,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="28.1071428571429"/>
-    <col collapsed="false" hidden="false" max="1025" min="2" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="27.8061224489796"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="12.5459183673469"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1064,333 +1475,405 @@
       <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>51</v>
-      </c>
-      <c r="B2" s="0" t="n">
+        <v>99</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>100</v>
+      </c>
+      <c r="C2" s="0" t="n">
         <v>40.4</v>
       </c>
-      <c r="C2" s="0" t="n">
+      <c r="D2" s="0" t="n">
         <v>-79.05</v>
       </c>
-      <c r="D2" s="0" t="n">
+      <c r="E2" s="0" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>52</v>
-      </c>
-      <c r="B3" s="0" t="n">
+        <v>101</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="C3" s="0" t="n">
         <v>34.95</v>
       </c>
-      <c r="C3" s="0" t="n">
+      <c r="D3" s="0" t="n">
         <v>-110.2</v>
       </c>
-      <c r="D3" s="0" t="n">
+      <c r="E3" s="0" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>53</v>
-      </c>
-      <c r="B4" s="0" t="n">
+        <v>103</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="C4" s="0" t="n">
         <v>45.9</v>
       </c>
-      <c r="C4" s="0" t="n">
+      <c r="D4" s="0" t="n">
         <v>-106.45</v>
       </c>
-      <c r="D4" s="0" t="n">
+      <c r="E4" s="0" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>54</v>
-      </c>
-      <c r="B5" s="0" t="n">
+        <v>105</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>106</v>
+      </c>
+      <c r="C5" s="0" t="n">
         <v>40.1</v>
       </c>
-      <c r="C5" s="0" t="n">
+      <c r="D5" s="0" t="n">
         <v>-76.55</v>
       </c>
-      <c r="D5" s="0" t="n">
+      <c r="E5" s="0" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>55</v>
-      </c>
-      <c r="B6" s="0" t="n">
+        <v>107</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="C6" s="0" t="n">
         <v>34.55</v>
       </c>
-      <c r="C6" s="0" t="n">
+      <c r="D6" s="0" t="n">
         <v>-109.2</v>
       </c>
-      <c r="D6" s="0" t="n">
+      <c r="E6" s="0" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>56</v>
-      </c>
-      <c r="B7" s="0" t="n">
+        <v>109</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>110</v>
+      </c>
+      <c r="C7" s="0" t="n">
         <v>40.5</v>
       </c>
-      <c r="C7" s="0" t="n">
+      <c r="D7" s="0" t="n">
         <v>-107.35</v>
       </c>
-      <c r="D7" s="0" t="n">
+      <c r="E7" s="0" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>57</v>
-      </c>
-      <c r="B8" s="0" t="n">
+        <v>111</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="C8" s="0" t="n">
         <v>28.95</v>
       </c>
-      <c r="C8" s="0" t="n">
+      <c r="D8" s="0" t="n">
         <v>-82.65</v>
       </c>
-      <c r="D8" s="0" t="n">
+      <c r="E8" s="0" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>58</v>
-      </c>
-      <c r="B9" s="0" t="n">
+        <v>113</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="C9" s="0" t="n">
         <v>36.75</v>
       </c>
-      <c r="C9" s="0" t="n">
+      <c r="D9" s="0" t="n">
         <v>-108.3</v>
       </c>
-      <c r="D9" s="0" t="n">
+      <c r="E9" s="0" t="n">
         <v>35</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>59</v>
-      </c>
-      <c r="B10" s="0" t="n">
+        <v>115</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>116</v>
+      </c>
+      <c r="C10" s="0" t="n">
         <v>40.55</v>
       </c>
-      <c r="C10" s="0" t="n">
+      <c r="D10" s="0" t="n">
         <v>-80.45</v>
       </c>
-      <c r="D10" s="0" t="n">
+      <c r="E10" s="0" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>60</v>
-      </c>
-      <c r="B11" s="0" t="n">
+        <v>117</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="C11" s="0" t="n">
         <v>37.95</v>
       </c>
-      <c r="C11" s="0" t="n">
+      <c r="D11" s="0" t="n">
         <v>-87</v>
       </c>
-      <c r="D11" s="0" t="n">
+      <c r="E11" s="0" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>61</v>
-      </c>
-      <c r="B12" s="0" t="n">
+        <v>119</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="C12" s="0" t="n">
         <v>39.85</v>
       </c>
-      <c r="C12" s="0" t="n">
+      <c r="D12" s="0" t="n">
         <v>-79.9</v>
       </c>
-      <c r="D12" s="0" t="n">
+      <c r="E12" s="0" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>62</v>
-      </c>
-      <c r="B13" s="0" t="n">
+        <v>121</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>122</v>
+      </c>
+      <c r="C13" s="0" t="n">
         <v>39.25</v>
       </c>
-      <c r="C13" s="0" t="n">
+      <c r="D13" s="0" t="n">
         <v>-111.1</v>
       </c>
-      <c r="D13" s="0" t="n">
+      <c r="E13" s="0" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="B14" s="0" t="n">
+        <v>123</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="C14" s="0" t="n">
         <v>39.55</v>
       </c>
-      <c r="C14" s="0" t="n">
+      <c r="D14" s="0" t="n">
         <v>-112.55</v>
       </c>
-      <c r="D14" s="0" t="n">
+      <c r="E14" s="0" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>64</v>
-      </c>
-      <c r="B15" s="0" t="n">
+        <v>125</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="C15" s="0" t="n">
         <v>41.75</v>
       </c>
-      <c r="C15" s="0" t="n">
+      <c r="D15" s="0" t="n">
         <v>-108.65</v>
       </c>
-      <c r="D15" s="0" t="n">
+      <c r="E15" s="0" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="B16" s="0" t="n">
+        <v>127</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>128</v>
+      </c>
+      <c r="C16" s="0" t="n">
         <v>39.85</v>
       </c>
-      <c r="C16" s="0" t="n">
+      <c r="D16" s="0" t="n">
         <v>-80.7</v>
       </c>
-      <c r="D16" s="0" t="n">
+      <c r="E16" s="0" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="B17" s="0" t="n">
+        <v>129</v>
+      </c>
+      <c r="B17" s="0" t="s">
+        <v>130</v>
+      </c>
+      <c r="C17" s="0" t="n">
         <v>36.05</v>
       </c>
-      <c r="C17" s="0" t="n">
+      <c r="D17" s="0" t="n">
         <v>-87.9</v>
       </c>
-      <c r="D17" s="0" t="n">
+      <c r="E17" s="0" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="B18" s="0" t="n">
+        <v>131</v>
+      </c>
+      <c r="B18" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="C18" s="0" t="n">
         <v>37.2</v>
       </c>
-      <c r="C18" s="0" t="n">
+      <c r="D18" s="0" t="n">
         <v>-88.75</v>
       </c>
-      <c r="D18" s="0" t="n">
+      <c r="E18" s="0" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>68</v>
-      </c>
-      <c r="B19" s="0" t="n">
+        <v>133</v>
+      </c>
+      <c r="B19" s="0" t="s">
+        <v>134</v>
+      </c>
+      <c r="C19" s="0" t="n">
         <v>42.1</v>
       </c>
-      <c r="C19" s="0" t="n">
+      <c r="D19" s="0" t="n">
         <v>-104.85</v>
       </c>
-      <c r="D19" s="0" t="n">
+      <c r="E19" s="0" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>69</v>
-      </c>
-      <c r="B20" s="0" t="n">
+        <v>135</v>
+      </c>
+      <c r="B20" s="0" t="s">
+        <v>136</v>
+      </c>
+      <c r="C20" s="0" t="n">
         <v>47.4</v>
       </c>
-      <c r="C20" s="0" t="n">
+      <c r="D20" s="0" t="n">
         <v>-101.35</v>
       </c>
-      <c r="D20" s="0" t="n">
+      <c r="E20" s="0" t="n">
         <v>35</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>70</v>
-      </c>
-      <c r="B21" s="0" t="n">
+        <v>137</v>
+      </c>
+      <c r="B21" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="C21" s="0" t="n">
         <v>35.6</v>
       </c>
-      <c r="C21" s="0" t="n">
+      <c r="D21" s="0" t="n">
         <v>-80.95</v>
       </c>
-      <c r="D21" s="0" t="n">
+      <c r="E21" s="0" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>71</v>
-      </c>
-      <c r="B22" s="0" t="n">
+        <v>139</v>
+      </c>
+      <c r="B22" s="0" t="s">
+        <v>140</v>
+      </c>
+      <c r="C22" s="0" t="n">
         <v>36.9</v>
       </c>
-      <c r="C22" s="0" t="n">
+      <c r="D22" s="0" t="n">
         <v>-111.35</v>
       </c>
-      <c r="D22" s="0" t="n">
+      <c r="E22" s="0" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>72</v>
-      </c>
-      <c r="B23" s="0" t="n">
+        <v>141</v>
+      </c>
+      <c r="B23" s="0" t="s">
+        <v>142</v>
+      </c>
+      <c r="C23" s="0" t="n">
         <v>29.8</v>
       </c>
-      <c r="C23" s="0" t="n">
+      <c r="D23" s="0" t="n">
         <v>-81.55</v>
       </c>
-      <c r="D23" s="0" t="n">
+      <c r="E23" s="0" t="n">
         <v>20</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>73</v>
-      </c>
-      <c r="B24" s="0" t="n">
+        <v>143</v>
+      </c>
+      <c r="B24" s="0" t="s">
+        <v>144</v>
+      </c>
+      <c r="C24" s="0" t="n">
         <v>40.9</v>
       </c>
-      <c r="C24" s="0" t="n">
+      <c r="D24" s="0" t="n">
         <v>-117</v>
       </c>
-      <c r="D24" s="0" t="n">
+      <c r="E24" s="0" t="n">
         <v>20</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -1403,15 +1886,17 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:D1"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.5204081632653"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="22.1275510204082"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="15.4591836734694"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.3418367346939"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1427,11 +1912,269 @@
       <c r="D1" s="0" t="s">
         <v>3</v>
       </c>
+      <c r="E1" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>44.35</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>-68.21</v>
+      </c>
+      <c r="E2" s="0" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>146</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>29.25</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>-103.25</v>
+      </c>
+      <c r="E3" s="0" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>42.94</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>-122.1</v>
+      </c>
+      <c r="E4" s="0" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="B5" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>36.24</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>-116.82</v>
+      </c>
+      <c r="E5" s="0" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>149</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>36.06</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>-112.14</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>150</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>35.68</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>-83.53</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>34.51</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>-93.05</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>153</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>48.1</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>-88.55</v>
+      </c>
+      <c r="E9" s="0" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>43.87</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>-103.46</v>
+      </c>
+      <c r="E10" s="0" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="B11" s="0" t="s">
+        <v>155</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>35.07</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>-109.78</v>
+      </c>
+      <c r="E11" s="0" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>156</v>
+      </c>
+      <c r="B12" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>-87</v>
+      </c>
+      <c r="E12" s="0" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="B13" s="0" t="s">
+        <v>158</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>38.53</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>-78.35</v>
+      </c>
+      <c r="E13" s="0" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>159</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>44.6</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>-110.5</v>
+      </c>
+      <c r="E14" s="0" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="B15" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>37.83</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>-119.5</v>
+      </c>
+      <c r="E15" s="0" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="B16" s="0" t="s">
+        <v>161</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>37.3</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>-113.05</v>
+      </c>
+      <c r="E16" s="0" t="n">
+        <v>40</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>